<commit_message>
cd cr + fibonacci
</commit_message>
<xml_diff>
--- a/instruction_set/instruction_set.xlsx
+++ b/instruction_set/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigne\OneDrive\Desktop\projects\dsm-processor-sim\instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214D5AF4-F714-48F3-B38D-0D9926942A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E36C3C-8C8C-4E3C-8887-F3EA1EAE8E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{46D14E4C-D724-4611-9C4B-F0C807E422CD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="441">
   <si>
     <t>Instruction</t>
   </si>
@@ -487,13 +487,7 @@
     <t>cr&lt;FL&gt;</t>
   </si>
   <si>
-    <t>RD,Lor,Dsp</t>
-  </si>
-  <si>
     <t>Epc,WR</t>
-  </si>
-  <si>
-    <t>Eor,Lpc,End</t>
   </si>
   <si>
     <t>returns to address on top of stack if flag is true</t>
@@ -511,16 +505,10 @@
     <t>if &lt;FL&gt; is 0, skip 4,5,6,7;      put address from PC to bus</t>
   </si>
   <si>
-    <t>load address into OR; decrement SP to location on top of stack</t>
-  </si>
-  <si>
     <t>if flag value is 1,  program jumps to given address xx</t>
   </si>
   <si>
     <t>if flag value is 1, program stores current address in stack and jumps to address in AR</t>
-  </si>
-  <si>
-    <t>put address from OR(taken from memory) onto bus</t>
   </si>
   <si>
     <t>if flag value is 1, program stores current address in stack and jumps to given address xx</t>
@@ -1368,6 +1356,15 @@
   <si>
     <t>1</t>
   </si>
+  <si>
+    <t>load address into AR; decrement SP to location on top of stack</t>
+  </si>
+  <si>
+    <t>RD,Lar,Dsp</t>
+  </si>
+  <si>
+    <t>put address from AR(taken from memory) onto bus</t>
+  </si>
 </sst>
 </file>
 
@@ -1953,8 +1950,8 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2450,7 +2447,7 @@
         <v>131</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>54</v>
@@ -2545,7 +2542,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>18</v>
@@ -3072,7 +3069,7 @@
         <v>133</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>134</v>
@@ -3158,7 +3155,7 @@
         <v>144</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>145</v>
@@ -3167,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F56" s="18" t="s">
         <v>143</v>
@@ -3190,10 +3187,10 @@
         <v>141</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>156</v>
+        <v>438</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>148</v>
+        <v>439</v>
       </c>
       <c r="H57" s="10"/>
     </row>
@@ -3223,13 +3220,13 @@
         <v>6</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H59" s="10"/>
     </row>
@@ -3241,13 +3238,13 @@
         <v>7</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>159</v>
+        <v>440</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>140</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="H60" s="10"/>
     </row>
@@ -3256,7 +3253,7 @@
         <v>147</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>146</v>
@@ -3265,7 +3262,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
@@ -3317,13 +3314,13 @@
         <v>6</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H64" s="10"/>
     </row>
@@ -3455,105 +3452,105 @@
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="AR1" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -6496,7 +6493,7 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -6897,7 +6894,7 @@
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -7298,7 +7295,7 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -7699,7 +7696,7 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -8100,7 +8097,7 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -8501,7 +8498,7 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -8902,7 +8899,7 @@
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -9303,7 +9300,7 @@
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -9704,7 +9701,7 @@
     </row>
     <row r="48" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A48" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -9972,7 +9969,7 @@
     </row>
     <row r="50" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -10240,7 +10237,7 @@
     </row>
     <row r="52" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A52" s="20" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -10508,7 +10505,7 @@
     </row>
     <row r="54" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A54" s="20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -10776,7 +10773,7 @@
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A56" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -11044,7 +11041,7 @@
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A58" s="20" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -11312,7 +11309,7 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A60" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -11580,7 +11577,7 @@
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A62" s="20" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -11848,7 +11845,7 @@
     </row>
     <row r="64" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A64" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
@@ -12116,7 +12113,7 @@
     </row>
     <row r="66" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -12384,7 +12381,7 @@
     </row>
     <row r="68" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A68" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
@@ -12652,7 +12649,7 @@
     </row>
     <row r="70" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A70" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -12920,7 +12917,7 @@
     </row>
     <row r="72" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A72" s="20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -13188,7 +13185,7 @@
     </row>
     <row r="74" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
@@ -13456,7 +13453,7 @@
     </row>
     <row r="76" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
@@ -13724,7 +13721,7 @@
     </row>
     <row r="78" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -13992,7 +13989,7 @@
     </row>
     <row r="80" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -14260,7 +14257,7 @@
     </row>
     <row r="82" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B82" s="1">
         <v>0</v>
@@ -14528,7 +14525,7 @@
     </row>
     <row r="84" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A84" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -14796,7 +14793,7 @@
     </row>
     <row r="86" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A86" s="20" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
@@ -15064,7 +15061,7 @@
     </row>
     <row r="88" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A88" s="20" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -15332,7 +15329,7 @@
     </row>
     <row r="90" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A90" s="20" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B90" s="1">
         <v>0</v>
@@ -15600,7 +15597,7 @@
     </row>
     <row r="92" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A92" s="20" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B92" s="1">
         <v>0</v>
@@ -15868,7 +15865,7 @@
     </row>
     <row r="94" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A94" s="20" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B94" s="1">
         <v>0</v>
@@ -16136,7 +16133,7 @@
     </row>
     <row r="96" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A96" s="20" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1">
         <v>0</v>
@@ -16404,7 +16401,7 @@
     </row>
     <row r="98" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A98" s="20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1">
         <v>0</v>
@@ -16672,7 +16669,7 @@
     </row>
     <row r="100" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A100" s="20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -16940,7 +16937,7 @@
     </row>
     <row r="102" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B102" s="1">
         <v>0</v>
@@ -17208,7 +17205,7 @@
     </row>
     <row r="104" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B104" s="1">
         <v>0</v>
@@ -17476,7 +17473,7 @@
     </row>
     <row r="106" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B106" s="1">
         <v>0</v>
@@ -17744,7 +17741,7 @@
     </row>
     <row r="108" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B108" s="1">
         <v>0</v>
@@ -18012,7 +18009,7 @@
     </row>
     <row r="110" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B110" s="1">
         <v>0</v>
@@ -18280,7 +18277,7 @@
     </row>
     <row r="112" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A112" s="20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B112" s="1">
         <v>0</v>
@@ -18548,7 +18545,7 @@
     </row>
     <row r="114" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B114" s="1">
         <v>0</v>
@@ -18816,7 +18813,7 @@
     </row>
     <row r="116" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B116" s="1">
         <v>0</v>
@@ -19084,7 +19081,7 @@
     </row>
     <row r="118" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B118" s="1">
         <v>0</v>
@@ -19352,7 +19349,7 @@
     </row>
     <row r="120" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B120" s="1">
         <v>0</v>
@@ -19620,7 +19617,7 @@
     </row>
     <row r="122" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A122" s="20" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B122" s="1">
         <v>0</v>
@@ -19888,7 +19885,7 @@
     </row>
     <row r="124" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A124" s="20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B124" s="1">
         <v>0</v>
@@ -20156,7 +20153,7 @@
     </row>
     <row r="126" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A126" s="20" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -20424,7 +20421,7 @@
     </row>
     <row r="128" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A128" s="20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B128" s="1">
         <v>0</v>
@@ -20692,7 +20689,7 @@
     </row>
     <row r="130" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A130" s="20" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B130" s="1">
         <v>0</v>
@@ -20960,7 +20957,7 @@
     </row>
     <row r="132" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A132" s="20" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
@@ -21228,7 +21225,7 @@
     </row>
     <row r="134" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A134" s="20" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
@@ -21496,7 +21493,7 @@
     </row>
     <row r="136" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A136" s="20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B136" s="1">
         <v>0</v>
@@ -21764,7 +21761,7 @@
     </row>
     <row r="138" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A138" s="20" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -22032,7 +22029,7 @@
     </row>
     <row r="140" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A140" s="20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B140" s="1">
         <v>0</v>
@@ -22300,7 +22297,7 @@
     </row>
     <row r="142" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A142" s="20" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B142" s="1">
         <v>0</v>
@@ -22568,7 +22565,7 @@
     </row>
     <row r="144" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A144" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B144" s="1">
         <v>0</v>
@@ -22836,7 +22833,7 @@
     </row>
     <row r="146" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B146" s="1">
         <v>0</v>
@@ -23104,7 +23101,7 @@
     </row>
     <row r="148" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A148" s="20" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B148" s="1">
         <v>0</v>
@@ -23372,7 +23369,7 @@
     </row>
     <row r="150" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A150" s="20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B150" s="1">
         <v>0</v>
@@ -23640,7 +23637,7 @@
     </row>
     <row r="152" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A152" s="20" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B152" s="1">
         <v>0</v>
@@ -23908,7 +23905,7 @@
     </row>
     <row r="154" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A154" s="20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B154" s="1">
         <v>0</v>
@@ -24176,7 +24173,7 @@
     </row>
     <row r="156" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A156" s="20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B156" s="1">
         <v>0</v>
@@ -24444,7 +24441,7 @@
     </row>
     <row r="158" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A158" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B158" s="1">
         <v>0</v>
@@ -24712,7 +24709,7 @@
     </row>
     <row r="160" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B160" s="1">
         <v>0</v>
@@ -24980,7 +24977,7 @@
     </row>
     <row r="162" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A162" s="20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B162" s="1">
         <v>0</v>
@@ -25248,7 +25245,7 @@
     </row>
     <row r="164" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A164" s="20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B164" s="1">
         <v>0</v>
@@ -25516,7 +25513,7 @@
     </row>
     <row r="166" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A166" s="20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B166" s="1">
         <v>0</v>
@@ -25784,7 +25781,7 @@
     </row>
     <row r="168" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A168" s="20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B168" s="1">
         <v>0</v>
@@ -26052,7 +26049,7 @@
     </row>
     <row r="170" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A170" s="20" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B170" s="1">
         <v>0</v>
@@ -26320,7 +26317,7 @@
     </row>
     <row r="172" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A172" s="20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B172" s="1">
         <v>0</v>
@@ -26588,7 +26585,7 @@
     </row>
     <row r="174" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A174" s="20" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B174" s="1">
         <v>0</v>
@@ -26856,7 +26853,7 @@
     </row>
     <row r="176" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A176" s="20" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B176" s="1">
         <v>0</v>
@@ -27124,7 +27121,7 @@
     </row>
     <row r="178" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A178" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B178" s="1">
         <v>0</v>
@@ -27392,7 +27389,7 @@
     </row>
     <row r="180" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A180" s="20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B180" s="1">
         <v>0</v>
@@ -27660,7 +27657,7 @@
     </row>
     <row r="182" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A182" s="20" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B182" s="1">
         <v>0</v>
@@ -27928,7 +27925,7 @@
     </row>
     <row r="184" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A184" s="20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B184" s="1">
         <v>0</v>
@@ -28196,7 +28193,7 @@
     </row>
     <row r="186" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A186" s="20" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B186" s="1">
         <v>0</v>
@@ -28464,7 +28461,7 @@
     </row>
     <row r="188" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A188" s="20" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B188" s="1">
         <v>0</v>
@@ -28732,7 +28729,7 @@
     </row>
     <row r="190" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A190" s="20" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B190" s="1">
         <v>0</v>
@@ -29000,7 +28997,7 @@
     </row>
     <row r="192" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A192" s="20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B192" s="1">
         <v>0</v>
@@ -29268,7 +29265,7 @@
     </row>
     <row r="194" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A194" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B194" s="1">
         <v>0</v>
@@ -29536,7 +29533,7 @@
     </row>
     <row r="196" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A196" s="20" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B196" s="1">
         <v>0</v>
@@ -29804,7 +29801,7 @@
     </row>
     <row r="198" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A198" s="20" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B198" s="1">
         <v>0</v>
@@ -30072,7 +30069,7 @@
     </row>
     <row r="200" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A200" s="20" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B200" s="1">
         <v>0</v>
@@ -30340,7 +30337,7 @@
     </row>
     <row r="202" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A202" s="20" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B202" s="1">
         <v>0</v>
@@ -30608,7 +30605,7 @@
     </row>
     <row r="204" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A204" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B204" s="1">
         <v>0</v>
@@ -30876,7 +30873,7 @@
     </row>
     <row r="206" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A206" s="20" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B206" s="1">
         <v>0</v>
@@ -31144,7 +31141,7 @@
     </row>
     <row r="208" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A208" s="20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B208" s="1">
         <v>0</v>
@@ -31412,7 +31409,7 @@
     </row>
     <row r="210" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A210" s="20" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B210" s="1">
         <v>0</v>
@@ -31680,7 +31677,7 @@
     </row>
     <row r="212" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A212" s="20" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B212" s="1">
         <v>0</v>
@@ -31948,7 +31945,7 @@
     </row>
     <row r="214" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A214" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B214" s="1">
         <v>0</v>
@@ -32216,7 +32213,7 @@
     </row>
     <row r="216" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A216" s="20" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B216" s="1">
         <v>0</v>
@@ -32484,7 +32481,7 @@
     </row>
     <row r="218" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A218" s="20" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B218" s="1">
         <v>0</v>
@@ -32752,7 +32749,7 @@
     </row>
     <row r="220" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A220" s="20" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B220" s="1">
         <v>0</v>
@@ -33020,7 +33017,7 @@
     </row>
     <row r="222" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A222" s="20" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B222" s="1">
         <v>0</v>
@@ -33288,7 +33285,7 @@
     </row>
     <row r="224" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A224" s="20" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B224" s="1">
         <v>0</v>
@@ -33556,7 +33553,7 @@
     </row>
     <row r="226" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A226" s="20" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B226" s="1">
         <v>0</v>
@@ -33824,7 +33821,7 @@
     </row>
     <row r="228" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A228" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B228" s="1">
         <v>0</v>
@@ -34092,7 +34089,7 @@
     </row>
     <row r="230" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A230" s="20" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B230" s="1">
         <v>0</v>
@@ -34360,7 +34357,7 @@
     </row>
     <row r="232" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A232" s="20" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B232" s="1">
         <v>0</v>
@@ -34628,7 +34625,7 @@
     </row>
     <row r="234" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A234" s="20" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B234" s="1">
         <v>0</v>
@@ -34896,7 +34893,7 @@
     </row>
     <row r="236" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A236" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B236" s="1">
         <v>0</v>
@@ -35164,7 +35161,7 @@
     </row>
     <row r="238" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A238" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B238" s="1">
         <v>0</v>
@@ -35432,7 +35429,7 @@
     </row>
     <row r="240" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A240" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B240" s="1">
         <v>0</v>
@@ -35567,7 +35564,7 @@
     </row>
     <row r="241" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A241" s="20" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B241" s="1">
         <v>0</v>
@@ -35702,7 +35699,7 @@
     </row>
     <row r="242" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A242" s="20" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B242" s="1">
         <v>0</v>
@@ -35837,7 +35834,7 @@
     </row>
     <row r="243" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A243" s="20" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B243" s="1">
         <v>0</v>
@@ -35972,7 +35969,7 @@
     </row>
     <row r="244" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A244" s="20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B244" s="1">
         <v>0</v>
@@ -36107,7 +36104,7 @@
     </row>
     <row r="245" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A245" s="20" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B245" s="1">
         <v>0</v>
@@ -36242,7 +36239,7 @@
     </row>
     <row r="246" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A246" s="20" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B246" s="1">
         <v>0</v>
@@ -36377,7 +36374,7 @@
     </row>
     <row r="247" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A247" s="20" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B247" s="1">
         <v>0</v>
@@ -36512,7 +36509,7 @@
     </row>
     <row r="248" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A248" s="20" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B248" s="1">
         <v>0</v>
@@ -36647,7 +36644,7 @@
     </row>
     <row r="249" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A249" s="20" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B249" s="1">
         <v>0</v>
@@ -36782,7 +36779,7 @@
     </row>
     <row r="250" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A250" s="20" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B250" s="1">
         <v>0</v>
@@ -36917,7 +36914,7 @@
     </row>
     <row r="251" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A251" s="20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B251" s="1">
         <v>0</v>
@@ -37052,7 +37049,7 @@
     </row>
     <row r="252" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A252" s="20" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B252" s="1">
         <v>0</v>
@@ -37187,7 +37184,7 @@
     </row>
     <row r="253" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A253" s="20" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B253" s="1">
         <v>0</v>
@@ -37322,7 +37319,7 @@
     </row>
     <row r="254" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A254" s="20" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B254" s="1">
         <v>0</v>
@@ -37457,7 +37454,7 @@
     </row>
     <row r="255" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A255" s="20" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B255" s="1">
         <v>0</v>
@@ -37592,7 +37589,7 @@
     </row>
     <row r="256" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A256" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B256" s="1">
         <v>0</v>
@@ -37727,7 +37724,7 @@
     </row>
     <row r="257" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A257" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B257" s="1">
         <v>0</v>
@@ -37862,7 +37859,7 @@
     </row>
     <row r="258" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B258" s="1">
         <v>0</v>
@@ -37997,7 +37994,7 @@
     </row>
     <row r="259" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A259" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B259" s="1">
         <v>0</v>
@@ -38132,7 +38129,7 @@
     </row>
     <row r="260" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A260" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B260" s="1">
         <v>0</v>
@@ -38267,7 +38264,7 @@
     </row>
     <row r="261" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A261" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B261" s="1">
         <v>0</v>
@@ -38402,7 +38399,7 @@
     </row>
     <row r="262" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A262" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B262" s="1">
         <v>0</v>
@@ -38537,7 +38534,7 @@
     </row>
     <row r="263" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A263" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B263" s="1">
         <v>0</v>
@@ -38672,7 +38669,7 @@
     </row>
     <row r="264" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A264" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B264" s="1">
         <v>0</v>
@@ -38807,7 +38804,7 @@
     </row>
     <row r="265" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B265" s="1">
         <v>0</v>
@@ -38942,7 +38939,7 @@
     </row>
     <row r="266" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A266" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B266" s="1">
         <v>0</v>
@@ -39077,7 +39074,7 @@
     </row>
     <row r="267" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B267" s="1">
         <v>0</v>
@@ -39212,7 +39209,7 @@
     </row>
     <row r="268" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B268" s="1">
         <v>0</v>
@@ -39347,7 +39344,7 @@
     </row>
     <row r="269" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B269" s="1">
         <v>0</v>
@@ -39482,7 +39479,7 @@
     </row>
     <row r="270" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B270" s="1">
         <v>0</v>
@@ -39617,7 +39614,7 @@
     </row>
     <row r="271" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B271" s="1">
         <v>0</v>
@@ -39752,7 +39749,7 @@
     </row>
     <row r="272" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B272" s="1">
         <v>0</v>
@@ -40019,7 +40016,7 @@
     </row>
     <row r="274" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B274" s="1">
         <v>0</v>
@@ -40286,7 +40283,7 @@
     </row>
     <row r="276" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B276" s="1">
         <v>0</v>
@@ -40553,7 +40550,7 @@
     </row>
     <row r="278" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B278" s="1">
         <v>0</v>
@@ -40820,7 +40817,7 @@
     </row>
     <row r="280" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A280" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B280" s="1">
         <v>0</v>
@@ -41087,7 +41084,7 @@
     </row>
     <row r="282" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B282" s="1">
         <v>0</v>
@@ -41354,7 +41351,7 @@
     </row>
     <row r="284" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B284" s="1">
         <v>0</v>
@@ -41621,7 +41618,7 @@
     </row>
     <row r="286" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B286" s="1">
         <v>0</v>
@@ -41888,7 +41885,7 @@
     </row>
     <row r="288" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B288" s="1">
         <v>0</v>
@@ -42155,7 +42152,7 @@
     </row>
     <row r="290" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B290" s="1">
         <v>0</v>
@@ -42422,7 +42419,7 @@
     </row>
     <row r="292" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B292" s="1">
         <v>0</v>
@@ -42689,7 +42686,7 @@
     </row>
     <row r="294" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B294" s="1">
         <v>0</v>
@@ -42956,7 +42953,7 @@
     </row>
     <row r="296" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A296" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B296" s="1">
         <v>0</v>
@@ -43223,7 +43220,7 @@
     </row>
     <row r="298" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A298" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B298" s="1">
         <v>0</v>
@@ -43490,7 +43487,7 @@
     </row>
     <row r="300" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A300" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B300" s="1">
         <v>0</v>
@@ -43757,7 +43754,7 @@
     </row>
     <row r="302" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B302" s="1">
         <v>0</v>
@@ -44024,7 +44021,7 @@
     </row>
     <row r="304" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A304" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B304" s="1">
         <v>0</v>
@@ -44291,7 +44288,7 @@
     </row>
     <row r="306" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B306" s="1">
         <v>0</v>
@@ -44558,7 +44555,7 @@
     </row>
     <row r="308" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A308" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B308" s="1">
         <v>0</v>
@@ -44825,7 +44822,7 @@
     </row>
     <row r="310" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A310" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B310" s="1">
         <v>0</v>
@@ -45092,7 +45089,7 @@
     </row>
     <row r="312" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A312" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B312" s="1">
         <v>0</v>
@@ -45359,7 +45356,7 @@
     </row>
     <row r="314" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A314" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B314" s="1">
         <v>0</v>
@@ -45626,7 +45623,7 @@
     </row>
     <row r="316" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A316" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B316" s="1">
         <v>0</v>
@@ -45893,7 +45890,7 @@
     </row>
     <row r="318" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A318" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B318" s="1">
         <v>0</v>
@@ -46160,7 +46157,7 @@
     </row>
     <row r="320" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A320" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B320" s="1">
         <v>0</v>
@@ -46427,7 +46424,7 @@
     </row>
     <row r="322" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B322" s="1">
         <v>0</v>
@@ -46694,7 +46691,7 @@
     </row>
     <row r="324" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A324" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B324" s="1">
         <v>0</v>
@@ -46961,7 +46958,7 @@
     </row>
     <row r="326" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A326" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B326" s="1">
         <v>0</v>
@@ -47228,7 +47225,7 @@
     </row>
     <row r="328" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B328" s="1">
         <v>0</v>
@@ -47495,7 +47492,7 @@
     </row>
     <row r="330" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B330" s="1">
         <v>0</v>
@@ -47762,7 +47759,7 @@
     </row>
     <row r="332" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A332" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B332" s="1">
         <v>0</v>
@@ -48029,7 +48026,7 @@
     </row>
     <row r="334" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A334" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B334" s="1">
         <v>0</v>
@@ -48296,7 +48293,7 @@
     </row>
     <row r="336" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B336" s="1">
         <v>0</v>
@@ -48563,7 +48560,7 @@
     </row>
     <row r="338" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A338" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B338" s="1">
         <v>0</v>
@@ -48830,7 +48827,7 @@
     </row>
     <row r="340" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A340" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B340" s="1">
         <v>0</v>
@@ -49097,7 +49094,7 @@
     </row>
     <row r="342" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A342" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B342" s="1">
         <v>0</v>
@@ -49364,7 +49361,7 @@
     </row>
     <row r="344" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B344" s="1">
         <v>0</v>
@@ -49631,7 +49628,7 @@
     </row>
     <row r="346" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B346" s="1">
         <v>0</v>
@@ -49898,7 +49895,7 @@
     </row>
     <row r="348" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B348" s="1">
         <v>0</v>
@@ -50165,7 +50162,7 @@
     </row>
     <row r="350" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B350" s="1">
         <v>0</v>
@@ -50432,7 +50429,7 @@
     </row>
     <row r="352" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A352" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B352" s="1">
         <v>0</v>
@@ -50699,7 +50696,7 @@
     </row>
     <row r="354" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A354" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B354" s="1">
         <v>0</v>
@@ -50966,7 +50963,7 @@
     </row>
     <row r="356" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A356" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B356" s="1">
         <v>0</v>
@@ -51233,7 +51230,7 @@
     </row>
     <row r="358" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B358" s="1">
         <v>0</v>
@@ -51500,7 +51497,7 @@
     </row>
     <row r="360" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A360" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B360" s="1">
         <v>0</v>
@@ -51767,7 +51764,7 @@
     </row>
     <row r="362" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A362" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B362" s="1">
         <v>0</v>
@@ -52034,7 +52031,7 @@
     </row>
     <row r="364" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A364" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B364" s="1">
         <v>0</v>
@@ -52301,7 +52298,7 @@
     </row>
     <row r="366" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B366" s="1">
         <v>0</v>
@@ -52568,7 +52565,7 @@
     </row>
     <row r="368" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A368" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B368" s="1">
         <v>0</v>
@@ -52967,7 +52964,7 @@
     </row>
     <row r="371" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A371" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B371" s="1">
         <v>0</v>
@@ -53368,7 +53365,7 @@
     </row>
     <row r="374" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A374" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B374" s="1">
         <v>0</v>
@@ -53769,7 +53766,7 @@
     </row>
     <row r="377" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A377" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B377" s="1">
         <v>0</v>
@@ -54170,7 +54167,7 @@
     </row>
     <row r="380" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B380" s="1">
         <v>0</v>
@@ -54571,7 +54568,7 @@
     </row>
     <row r="383" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A383" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B383" s="1">
         <v>0</v>
@@ -54972,7 +54969,7 @@
     </row>
     <row r="386" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A386" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B386" s="1">
         <v>0</v>
@@ -55373,7 +55370,7 @@
     </row>
     <row r="389" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B389" s="1">
         <v>0</v>
@@ -55774,7 +55771,7 @@
     </row>
     <row r="392" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A392" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B392" s="1">
         <v>0</v>
@@ -56175,7 +56172,7 @@
     </row>
     <row r="395" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B395" s="1">
         <v>0</v>
@@ -56576,7 +56573,7 @@
     </row>
     <row r="398" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B398" s="1">
         <v>0</v>
@@ -56977,7 +56974,7 @@
     </row>
     <row r="401" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A401" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B401" s="1">
         <v>0</v>
@@ -57378,7 +57375,7 @@
     </row>
     <row r="404" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A404" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B404" s="1">
         <v>0</v>
@@ -57779,7 +57776,7 @@
     </row>
     <row r="407" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A407" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B407" s="1">
         <v>0</v>
@@ -58180,7 +58177,7 @@
     </row>
     <row r="410" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A410" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B410" s="1">
         <v>0</v>
@@ -58581,7 +58578,7 @@
     </row>
     <row r="413" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A413" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B413" s="1">
         <v>0</v>
@@ -58982,7 +58979,7 @@
     </row>
     <row r="416" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A416" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B416" s="1">
         <v>0</v>
@@ -59249,7 +59246,7 @@
     </row>
     <row r="418" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A418" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B418" s="1">
         <v>0</v>
@@ -59516,7 +59513,7 @@
     </row>
     <row r="420" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A420" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B420" s="1">
         <v>0</v>
@@ -59783,7 +59780,7 @@
     </row>
     <row r="422" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A422" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B422" s="1">
         <v>0</v>
@@ -60050,7 +60047,7 @@
     </row>
     <row r="424" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A424" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B424" s="1">
         <v>0</v>
@@ -60317,7 +60314,7 @@
     </row>
     <row r="426" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A426" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B426" s="1">
         <v>0</v>
@@ -60584,7 +60581,7 @@
     </row>
     <row r="428" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A428" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B428" s="1">
         <v>0</v>
@@ -60851,7 +60848,7 @@
     </row>
     <row r="430" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A430" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B430" s="1">
         <v>0</v>
@@ -61118,7 +61115,7 @@
     </row>
     <row r="432" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A432" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B432" s="1">
         <v>0</v>
@@ -61385,7 +61382,7 @@
     </row>
     <row r="434" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A434" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B434" s="1">
         <v>0</v>
@@ -61652,7 +61649,7 @@
     </row>
     <row r="436" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A436" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B436" s="1">
         <v>0</v>
@@ -61919,7 +61916,7 @@
     </row>
     <row r="438" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A438" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B438" s="1">
         <v>0</v>
@@ -62186,7 +62183,7 @@
     </row>
     <row r="440" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A440" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B440" s="1">
         <v>0</v>
@@ -62453,7 +62450,7 @@
     </row>
     <row r="442" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A442" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B442" s="1">
         <v>0</v>
@@ -62720,7 +62717,7 @@
     </row>
     <row r="444" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A444" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B444" s="1">
         <v>0</v>
@@ -62987,7 +62984,7 @@
     </row>
     <row r="446" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A446" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B446" s="1">
         <v>0</v>
@@ -63254,7 +63251,7 @@
     </row>
     <row r="448" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A448" s="20" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B448" s="1">
         <v>0</v>
@@ -63522,7 +63519,7 @@
     </row>
     <row r="450" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A450" s="20" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B450" s="1">
         <v>0</v>
@@ -63790,7 +63787,7 @@
     </row>
     <row r="452" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A452" s="20" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B452" s="1">
         <v>0</v>
@@ -64058,7 +64055,7 @@
     </row>
     <row r="454" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A454" s="20" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B454" s="1">
         <v>0</v>
@@ -64326,7 +64323,7 @@
     </row>
     <row r="456" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A456" s="20" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B456" s="1">
         <v>0</v>
@@ -64594,7 +64591,7 @@
     </row>
     <row r="458" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A458" s="20" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B458" s="1">
         <v>0</v>
@@ -64862,7 +64859,7 @@
     </row>
     <row r="460" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A460" s="20" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B460" s="1">
         <v>0</v>
@@ -65130,7 +65127,7 @@
     </row>
     <row r="462" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A462" s="20" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B462" s="1">
         <v>0</v>
@@ -65398,7 +65395,7 @@
     </row>
     <row r="464" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A464" s="20" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B464" s="1">
         <v>0</v>
@@ -65666,7 +65663,7 @@
     </row>
     <row r="466" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A466" s="20" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B466" s="1">
         <v>0</v>
@@ -65934,7 +65931,7 @@
     </row>
     <row r="468" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A468" s="20" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B468" s="1">
         <v>0</v>
@@ -66202,7 +66199,7 @@
     </row>
     <row r="470" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A470" s="20" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B470" s="1">
         <v>0</v>
@@ -66470,7 +66467,7 @@
     </row>
     <row r="472" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A472" s="20" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B472" s="1">
         <v>0</v>
@@ -66738,7 +66735,7 @@
     </row>
     <row r="474" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A474" s="20" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B474" s="1">
         <v>0</v>
@@ -67006,7 +67003,7 @@
     </row>
     <row r="476" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A476" s="20" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B476" s="1">
         <v>0</v>
@@ -67274,7 +67271,7 @@
     </row>
     <row r="478" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A478" s="20" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B478" s="1">
         <v>0</v>
@@ -67542,7 +67539,7 @@
     </row>
     <row r="480" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A480" s="20" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B480" s="1">
         <v>0</v>
@@ -68209,7 +68206,7 @@
     </row>
     <row r="485" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A485" s="20" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B485" s="1">
         <v>0</v>
@@ -68876,7 +68873,7 @@
     </row>
     <row r="490" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A490" s="20" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B490" s="1">
         <v>0</v>
@@ -69543,7 +69540,7 @@
     </row>
     <row r="495" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A495" s="20" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B495" s="1">
         <v>0</v>
@@ -70210,7 +70207,7 @@
     </row>
     <row r="500" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A500" s="20" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B500" s="1">
         <v>0</v>
@@ -70877,7 +70874,7 @@
     </row>
     <row r="505" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A505" s="20" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B505" s="1">
         <v>0</v>
@@ -71544,7 +71541,7 @@
     </row>
     <row r="510" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A510" s="20" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B510" s="1">
         <v>0</v>
@@ -72211,7 +72208,7 @@
     </row>
     <row r="515" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A515" s="20" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B515" s="1">
         <v>1</v>
@@ -72878,7 +72875,7 @@
     </row>
     <row r="520" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A520" s="20" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B520" s="1">
         <v>1</v>
@@ -73544,7 +73541,7 @@
     </row>
     <row r="525" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A525" s="20" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B525" s="1">
         <v>1</v>
@@ -74210,7 +74207,7 @@
     </row>
     <row r="530" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A530" s="20" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B530" s="1">
         <v>1</v>
@@ -74876,7 +74873,7 @@
     </row>
     <row r="535" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A535" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B535" s="1">
         <v>1</v>
@@ -75542,7 +75539,7 @@
     </row>
     <row r="540" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A540" s="20" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B540" s="1">
         <v>1</v>
@@ -76208,7 +76205,7 @@
     </row>
     <row r="545" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A545" s="20" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B545" s="1">
         <v>1</v>
@@ -76874,7 +76871,7 @@
     </row>
     <row r="550" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A550" s="20" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B550" s="1">
         <v>1</v>
@@ -77540,7 +77537,7 @@
     </row>
     <row r="555" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A555" s="20" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B555" s="1">
         <v>1</v>
@@ -78228,7 +78225,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B1">
         <v>2</v>
@@ -78263,7 +78260,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -79043,7 +79040,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -79148,7 +79145,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -79253,7 +79250,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -79358,7 +79355,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -79463,7 +79460,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -79568,7 +79565,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -79673,7 +79670,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -79778,7 +79775,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -79883,7 +79880,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -79955,7 +79952,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -80027,7 +80024,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="20" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -80099,7 +80096,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -80171,7 +80168,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -80243,7 +80240,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="20" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -80315,7 +80312,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -80387,7 +80384,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="20" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -80459,7 +80456,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
@@ -80531,7 +80528,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -80603,7 +80600,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
@@ -80675,7 +80672,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -80747,7 +80744,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -80819,7 +80816,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
@@ -80891,7 +80888,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
@@ -80963,7 +80960,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -81035,7 +81032,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -81107,7 +81104,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B82" s="1">
         <v>0</v>
@@ -81179,7 +81176,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -81251,7 +81248,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="20" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
@@ -81323,7 +81320,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="20" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -81395,7 +81392,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="20" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B90" s="1">
         <v>0</v>
@@ -81467,7 +81464,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="20" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B92" s="1">
         <v>0</v>
@@ -81539,7 +81536,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="20" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B94" s="1">
         <v>0</v>
@@ -81611,7 +81608,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="20" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1">
         <v>0</v>
@@ -81683,7 +81680,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1">
         <v>0</v>
@@ -81755,7 +81752,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -81827,7 +81824,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B102" s="1">
         <v>0</v>
@@ -81899,7 +81896,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B104" s="1">
         <v>0</v>
@@ -81971,7 +81968,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B106" s="1">
         <v>0</v>
@@ -82043,7 +82040,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B108" s="1">
         <v>0</v>
@@ -82115,7 +82112,7 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B110" s="1">
         <v>0</v>
@@ -82187,7 +82184,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B112" s="1">
         <v>0</v>
@@ -82259,7 +82256,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B114" s="1">
         <v>0</v>
@@ -82331,7 +82328,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B116" s="1">
         <v>0</v>
@@ -82403,7 +82400,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B118" s="1">
         <v>0</v>
@@ -82475,7 +82472,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B120" s="1">
         <v>0</v>
@@ -82547,7 +82544,7 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="20" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B122" s="1">
         <v>0</v>
@@ -82619,7 +82616,7 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B124" s="1">
         <v>0</v>
@@ -82691,7 +82688,7 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="20" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -82763,7 +82760,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B128" s="1">
         <v>0</v>
@@ -82835,7 +82832,7 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="20" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B130" s="1">
         <v>0</v>
@@ -82907,7 +82904,7 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="20" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
@@ -82979,7 +82976,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="20" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
@@ -83051,7 +83048,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B136" s="1">
         <v>0</v>
@@ -83123,7 +83120,7 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="20" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -83195,7 +83192,7 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B140" s="1">
         <v>0</v>
@@ -83267,7 +83264,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="20" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B142" s="1">
         <v>0</v>
@@ -83339,7 +83336,7 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B144" s="1">
         <v>0</v>
@@ -83411,7 +83408,7 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B146" s="1">
         <v>0</v>
@@ -83483,7 +83480,7 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="20" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B148" s="1">
         <v>0</v>
@@ -83555,7 +83552,7 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B150" s="1">
         <v>0</v>
@@ -83627,7 +83624,7 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="20" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B152" s="1">
         <v>0</v>
@@ -83699,7 +83696,7 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B154" s="1">
         <v>0</v>
@@ -83771,7 +83768,7 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B156" s="1">
         <v>0</v>
@@ -83843,7 +83840,7 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B158" s="1">
         <v>0</v>
@@ -83915,7 +83912,7 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B160" s="1">
         <v>0</v>
@@ -83987,7 +83984,7 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B162" s="1">
         <v>0</v>
@@ -84059,7 +84056,7 @@
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B164" s="1">
         <v>0</v>
@@ -84131,7 +84128,7 @@
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B166" s="1">
         <v>0</v>
@@ -84203,7 +84200,7 @@
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B168" s="1">
         <v>0</v>
@@ -84275,7 +84272,7 @@
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="20" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B170" s="1">
         <v>0</v>
@@ -84347,7 +84344,7 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B172" s="1">
         <v>0</v>
@@ -84419,7 +84416,7 @@
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="20" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B174" s="1">
         <v>0</v>
@@ -84491,7 +84488,7 @@
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="20" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B176" s="1">
         <v>0</v>
@@ -84563,7 +84560,7 @@
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B178" s="1">
         <v>0</v>
@@ -84635,7 +84632,7 @@
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B180" s="1">
         <v>0</v>
@@ -84707,7 +84704,7 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="20" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B182" s="1">
         <v>0</v>
@@ -84779,7 +84776,7 @@
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B184" s="1">
         <v>0</v>
@@ -84851,7 +84848,7 @@
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="20" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B186" s="1">
         <v>0</v>
@@ -84923,7 +84920,7 @@
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="20" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B188" s="1">
         <v>0</v>
@@ -84995,7 +84992,7 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="20" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B190" s="1">
         <v>0</v>
@@ -85067,7 +85064,7 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B192" s="1">
         <v>0</v>
@@ -85139,7 +85136,7 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B194" s="1">
         <v>0</v>
@@ -85211,7 +85208,7 @@
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="20" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B196" s="1">
         <v>0</v>
@@ -85283,7 +85280,7 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="20" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B198" s="1">
         <v>0</v>
@@ -85355,7 +85352,7 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="20" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B200" s="1">
         <v>0</v>
@@ -85427,7 +85424,7 @@
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="20" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B202" s="1">
         <v>0</v>
@@ -85499,7 +85496,7 @@
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B204" s="1">
         <v>0</v>
@@ -85571,7 +85568,7 @@
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="20" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B206" s="1">
         <v>0</v>
@@ -85643,7 +85640,7 @@
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B208" s="1">
         <v>0</v>
@@ -85715,7 +85712,7 @@
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="20" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B210" s="1">
         <v>0</v>
@@ -85787,7 +85784,7 @@
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" s="20" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B212" s="1">
         <v>0</v>
@@ -85859,7 +85856,7 @@
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B214" s="1">
         <v>0</v>
@@ -85931,7 +85928,7 @@
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" s="20" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B216" s="1">
         <v>0</v>
@@ -86003,7 +86000,7 @@
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" s="20" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B218" s="1">
         <v>0</v>
@@ -86075,7 +86072,7 @@
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" s="20" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B220" s="1">
         <v>0</v>
@@ -86147,7 +86144,7 @@
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" s="20" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B222" s="1">
         <v>0</v>
@@ -86219,7 +86216,7 @@
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" s="20" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B224" s="1">
         <v>0</v>
@@ -86291,7 +86288,7 @@
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" s="20" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B226" s="1">
         <v>0</v>
@@ -86363,7 +86360,7 @@
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B228" s="1">
         <v>0</v>
@@ -86435,7 +86432,7 @@
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" s="20" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B230" s="1">
         <v>0</v>
@@ -86507,7 +86504,7 @@
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" s="20" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B232" s="1">
         <v>0</v>
@@ -86579,7 +86576,7 @@
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" s="20" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B234" s="1">
         <v>0</v>
@@ -86651,7 +86648,7 @@
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B236" s="1">
         <v>0</v>
@@ -86723,7 +86720,7 @@
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B238" s="1">
         <v>0</v>
@@ -86795,7 +86792,7 @@
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B240" s="1">
         <v>0</v>
@@ -86834,7 +86831,7 @@
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" s="20" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B241" s="1">
         <v>0</v>
@@ -86873,7 +86870,7 @@
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" s="20" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B242" s="1">
         <v>0</v>
@@ -86912,7 +86909,7 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" s="20" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B243" s="1">
         <v>0</v>
@@ -86951,7 +86948,7 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" s="20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B244" s="1">
         <v>0</v>
@@ -86990,7 +86987,7 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" s="20" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B245" s="1">
         <v>0</v>
@@ -87029,7 +87026,7 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" s="20" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B246" s="1">
         <v>0</v>
@@ -87068,7 +87065,7 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" s="20" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B247" s="1">
         <v>0</v>
@@ -87107,7 +87104,7 @@
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" s="20" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B248" s="1">
         <v>0</v>
@@ -87146,7 +87143,7 @@
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" s="20" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B249" s="1">
         <v>0</v>
@@ -87185,7 +87182,7 @@
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" s="20" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B250" s="1">
         <v>0</v>
@@ -87224,7 +87221,7 @@
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" s="20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B251" s="1">
         <v>0</v>
@@ -87263,7 +87260,7 @@
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" s="20" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B252" s="1">
         <v>0</v>
@@ -87302,7 +87299,7 @@
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" s="20" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B253" s="1">
         <v>0</v>
@@ -87341,7 +87338,7 @@
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" s="20" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B254" s="1">
         <v>0</v>
@@ -87380,7 +87377,7 @@
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" s="20" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B255" s="1">
         <v>0</v>
@@ -87419,7 +87416,7 @@
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B256" s="1">
         <v>0</v>
@@ -87458,7 +87455,7 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B257" s="1">
         <v>0</v>
@@ -87497,7 +87494,7 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B258" s="1">
         <v>0</v>
@@ -87536,7 +87533,7 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B259" s="1">
         <v>0</v>
@@ -87575,7 +87572,7 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B260" s="1">
         <v>0</v>
@@ -87614,7 +87611,7 @@
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B261" s="1">
         <v>0</v>
@@ -87653,7 +87650,7 @@
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B262" s="1">
         <v>0</v>
@@ -87692,7 +87689,7 @@
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B263" s="1">
         <v>0</v>
@@ -87731,7 +87728,7 @@
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B264" s="1">
         <v>0</v>
@@ -87770,7 +87767,7 @@
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B265" s="1">
         <v>0</v>
@@ -87809,7 +87806,7 @@
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B266" s="1">
         <v>0</v>
@@ -87848,7 +87845,7 @@
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B267" s="1">
         <v>0</v>
@@ -87887,7 +87884,7 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B268" s="1">
         <v>0</v>
@@ -87926,7 +87923,7 @@
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B269" s="1">
         <v>0</v>
@@ -87965,7 +87962,7 @@
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B270" s="1">
         <v>0</v>
@@ -88004,7 +88001,7 @@
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B271" s="1">
         <v>0</v>
@@ -88043,7 +88040,7 @@
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B272" s="1">
         <v>0</v>
@@ -88115,7 +88112,7 @@
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B274" s="1">
         <v>0</v>
@@ -88187,7 +88184,7 @@
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B276" s="1">
         <v>0</v>
@@ -88259,7 +88256,7 @@
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B278" s="1">
         <v>0</v>
@@ -88331,7 +88328,7 @@
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B280" s="1">
         <v>0</v>
@@ -88403,7 +88400,7 @@
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B282" s="1">
         <v>0</v>
@@ -88475,7 +88472,7 @@
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B284" s="1">
         <v>0</v>
@@ -88547,7 +88544,7 @@
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B286" s="1">
         <v>0</v>
@@ -88619,7 +88616,7 @@
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B288" s="1">
         <v>0</v>
@@ -88691,7 +88688,7 @@
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B290" s="1">
         <v>0</v>
@@ -88763,7 +88760,7 @@
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B292" s="1">
         <v>0</v>
@@ -88835,7 +88832,7 @@
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B294" s="1">
         <v>0</v>
@@ -88907,7 +88904,7 @@
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B296" s="1">
         <v>0</v>
@@ -88979,7 +88976,7 @@
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B298" s="1">
         <v>0</v>
@@ -89051,7 +89048,7 @@
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B300" s="1">
         <v>0</v>
@@ -89123,7 +89120,7 @@
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B302" s="1">
         <v>0</v>
@@ -89195,7 +89192,7 @@
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B304" s="1">
         <v>0</v>
@@ -89267,7 +89264,7 @@
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B306" s="1">
         <v>0</v>
@@ -89339,7 +89336,7 @@
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B308" s="1">
         <v>0</v>
@@ -89411,7 +89408,7 @@
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B310" s="1">
         <v>0</v>
@@ -89483,7 +89480,7 @@
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B312" s="1">
         <v>0</v>
@@ -89555,7 +89552,7 @@
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A314" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B314" s="1">
         <v>0</v>
@@ -89627,7 +89624,7 @@
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A316" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B316" s="1">
         <v>0</v>
@@ -89699,7 +89696,7 @@
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A318" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B318" s="1">
         <v>0</v>
@@ -89771,7 +89768,7 @@
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A320" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B320" s="1">
         <v>0</v>
@@ -89843,7 +89840,7 @@
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B322" s="1">
         <v>0</v>
@@ -89915,7 +89912,7 @@
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A324" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B324" s="1">
         <v>0</v>
@@ -89987,7 +89984,7 @@
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A326" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B326" s="1">
         <v>0</v>
@@ -90059,7 +90056,7 @@
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B328" s="1">
         <v>0</v>
@@ -90131,7 +90128,7 @@
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B330" s="1">
         <v>0</v>
@@ -90203,7 +90200,7 @@
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A332" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B332" s="1">
         <v>0</v>
@@ -90275,7 +90272,7 @@
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A334" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B334" s="1">
         <v>0</v>
@@ -90347,7 +90344,7 @@
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B336" s="1">
         <v>0</v>
@@ -90419,7 +90416,7 @@
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A338" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B338" s="1">
         <v>0</v>
@@ -90491,7 +90488,7 @@
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A340" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B340" s="1">
         <v>0</v>
@@ -90563,7 +90560,7 @@
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A342" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B342" s="1">
         <v>0</v>
@@ -90635,7 +90632,7 @@
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B344" s="1">
         <v>0</v>
@@ -90707,7 +90704,7 @@
     </row>
     <row r="346" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B346" s="1">
         <v>0</v>
@@ -90779,7 +90776,7 @@
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B348" s="1">
         <v>0</v>
@@ -90851,7 +90848,7 @@
     </row>
     <row r="350" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B350" s="1">
         <v>0</v>
@@ -90923,7 +90920,7 @@
     </row>
     <row r="352" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A352" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B352" s="1">
         <v>0</v>
@@ -90995,7 +90992,7 @@
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A354" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B354" s="1">
         <v>0</v>
@@ -91067,7 +91064,7 @@
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A356" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B356" s="1">
         <v>0</v>
@@ -91139,7 +91136,7 @@
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B358" s="1">
         <v>0</v>
@@ -91211,7 +91208,7 @@
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A360" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B360" s="1">
         <v>0</v>
@@ -91283,7 +91280,7 @@
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A362" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B362" s="1">
         <v>0</v>
@@ -91355,7 +91352,7 @@
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A364" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B364" s="1">
         <v>0</v>
@@ -91427,7 +91424,7 @@
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B366" s="1">
         <v>0</v>
@@ -91499,7 +91496,7 @@
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A368" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B368" s="1">
         <v>0</v>
@@ -91604,7 +91601,7 @@
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A371" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B371" s="1">
         <v>0</v>
@@ -91709,7 +91706,7 @@
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A374" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B374" s="1">
         <v>0</v>
@@ -91814,7 +91811,7 @@
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A377" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B377" s="1">
         <v>0</v>
@@ -91919,7 +91916,7 @@
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B380" s="1">
         <v>0</v>
@@ -92024,7 +92021,7 @@
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A383" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B383" s="1">
         <v>0</v>
@@ -92129,7 +92126,7 @@
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A386" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B386" s="1">
         <v>0</v>
@@ -92234,7 +92231,7 @@
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B389" s="1">
         <v>0</v>
@@ -92339,7 +92336,7 @@
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A392" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B392" s="1">
         <v>0</v>
@@ -92444,7 +92441,7 @@
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B395" s="1">
         <v>0</v>
@@ -92549,7 +92546,7 @@
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B398" s="1">
         <v>0</v>
@@ -92654,7 +92651,7 @@
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A401" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B401" s="1">
         <v>0</v>
@@ -92759,7 +92756,7 @@
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A404" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B404" s="1">
         <v>0</v>
@@ -92864,7 +92861,7 @@
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A407" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B407" s="1">
         <v>0</v>
@@ -92969,7 +92966,7 @@
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A410" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B410" s="1">
         <v>0</v>
@@ -93074,7 +93071,7 @@
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A413" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B413" s="1">
         <v>0</v>
@@ -93179,7 +93176,7 @@
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A416" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B416" s="1">
         <v>0</v>
@@ -93251,7 +93248,7 @@
     </row>
     <row r="418" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A418" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B418" s="1">
         <v>0</v>
@@ -93323,7 +93320,7 @@
     </row>
     <row r="420" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A420" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B420" s="1">
         <v>0</v>
@@ -93395,7 +93392,7 @@
     </row>
     <row r="422" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A422" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B422" s="1">
         <v>0</v>
@@ -93467,7 +93464,7 @@
     </row>
     <row r="424" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A424" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B424" s="1">
         <v>0</v>
@@ -93539,7 +93536,7 @@
     </row>
     <row r="426" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A426" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B426" s="1">
         <v>0</v>
@@ -93611,7 +93608,7 @@
     </row>
     <row r="428" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A428" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B428" s="1">
         <v>0</v>
@@ -93683,7 +93680,7 @@
     </row>
     <row r="430" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A430" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B430" s="1">
         <v>0</v>
@@ -93755,7 +93752,7 @@
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A432" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B432" s="1">
         <v>0</v>
@@ -93827,7 +93824,7 @@
     </row>
     <row r="434" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A434" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B434" s="1">
         <v>0</v>
@@ -93899,7 +93896,7 @@
     </row>
     <row r="436" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A436" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B436" s="1">
         <v>0</v>
@@ -93971,7 +93968,7 @@
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A438" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B438" s="1">
         <v>0</v>
@@ -94043,7 +94040,7 @@
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A440" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B440" s="1">
         <v>0</v>
@@ -94115,7 +94112,7 @@
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A442" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B442" s="1">
         <v>0</v>
@@ -94187,7 +94184,7 @@
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A444" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B444" s="1">
         <v>0</v>
@@ -94259,7 +94256,7 @@
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A446" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B446" s="1">
         <v>0</v>
@@ -94331,7 +94328,7 @@
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A448" s="20" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B448" s="1">
         <v>0</v>
@@ -94403,7 +94400,7 @@
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A450" s="20" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B450" s="1">
         <v>0</v>
@@ -94475,7 +94472,7 @@
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A452" s="20" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B452" s="1">
         <v>0</v>
@@ -94547,7 +94544,7 @@
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A454" s="20" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B454" s="1">
         <v>0</v>
@@ -94619,7 +94616,7 @@
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A456" s="20" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B456" s="1">
         <v>0</v>
@@ -94691,7 +94688,7 @@
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A458" s="20" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B458" s="1">
         <v>0</v>
@@ -94763,7 +94760,7 @@
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A460" s="20" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B460" s="1">
         <v>0</v>
@@ -94835,7 +94832,7 @@
     </row>
     <row r="462" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A462" s="20" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B462" s="1">
         <v>0</v>
@@ -94907,7 +94904,7 @@
     </row>
     <row r="464" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A464" s="20" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B464" s="1">
         <v>0</v>
@@ -94979,7 +94976,7 @@
     </row>
     <row r="466" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A466" s="20" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B466" s="1">
         <v>0</v>
@@ -95051,7 +95048,7 @@
     </row>
     <row r="468" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A468" s="20" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B468" s="1">
         <v>0</v>
@@ -95123,7 +95120,7 @@
     </row>
     <row r="470" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A470" s="20" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B470" s="1">
         <v>0</v>
@@ -95195,7 +95192,7 @@
     </row>
     <row r="472" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A472" s="20" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B472" s="1">
         <v>0</v>
@@ -95267,7 +95264,7 @@
     </row>
     <row r="474" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A474" s="20" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B474" s="1">
         <v>0</v>
@@ -95339,7 +95336,7 @@
     </row>
     <row r="476" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A476" s="20" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B476" s="1">
         <v>0</v>
@@ -95411,7 +95408,7 @@
     </row>
     <row r="478" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A478" s="20" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B478" s="1">
         <v>0</v>
@@ -95483,7 +95480,7 @@
     </row>
     <row r="480" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A480" s="20" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B480" s="1">
         <v>0</v>
@@ -95654,7 +95651,7 @@
     </row>
     <row r="485" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A485" s="20" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B485" s="1">
         <v>0</v>
@@ -95825,7 +95822,7 @@
     </row>
     <row r="490" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A490" s="20" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B490" s="1">
         <v>0</v>
@@ -95996,7 +95993,7 @@
     </row>
     <row r="495" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A495" s="20" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B495" s="1">
         <v>0</v>
@@ -96167,7 +96164,7 @@
     </row>
     <row r="500" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A500" s="20" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B500" s="1">
         <v>0</v>
@@ -96338,7 +96335,7 @@
     </row>
     <row r="505" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A505" s="20" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B505" s="1">
         <v>0</v>
@@ -96509,7 +96506,7 @@
     </row>
     <row r="510" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A510" s="20" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B510" s="1">
         <v>0</v>
@@ -96680,7 +96677,7 @@
     </row>
     <row r="515" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A515" s="20" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B515" s="1">
         <v>1</v>
@@ -96851,7 +96848,7 @@
     </row>
     <row r="520" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A520" s="20" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B520" s="1">
         <v>1</v>
@@ -97022,7 +97019,7 @@
     </row>
     <row r="525" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A525" s="20" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B525" s="1">
         <v>1</v>
@@ -97193,7 +97190,7 @@
     </row>
     <row r="530" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A530" s="20" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B530" s="1">
         <v>1</v>
@@ -97364,7 +97361,7 @@
     </row>
     <row r="535" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A535" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B535" s="1">
         <v>1</v>
@@ -97535,7 +97532,7 @@
     </row>
     <row r="540" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A540" s="20" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B540" s="1">
         <v>1</v>
@@ -97706,7 +97703,7 @@
     </row>
     <row r="545" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A545" s="20" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B545" s="1">
         <v>1</v>
@@ -97877,7 +97874,7 @@
     </row>
     <row r="550" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A550" s="20" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B550" s="1">
         <v>1</v>
@@ -98048,7 +98045,7 @@
     </row>
     <row r="555" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A555" s="20" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B555" s="1">
         <v>1</v>

</xml_diff>